<commit_message>
Add presentation for DTF, re-run forecast
</commit_message>
<xml_diff>
--- a/data/final_dtf_rmse.xlsx
+++ b/data/final_dtf_rmse.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/29mob/ltd_forecasting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605C452D-6717-304B-BF6D-F717DF5E9E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9664B2-E4B2-404B-8808-6ECE84C274A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
     <sheet name="forecasts (all sa)" sheetId="1" r:id="rId2"/>
     <sheet name="forecasts (all origional)" sheetId="3" r:id="rId3"/>
     <sheet name="rmse" sheetId="4" r:id="rId4"/>
+    <sheet name="mape" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.4" hidden="1">'forecasts (all origional)'!$AM$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'forecasts (all origional)'!$AM$2:$AM$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'forecasts (all origional)'!$AN$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'forecasts (all origional)'!$AN$2:$AN$13</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">'forecasts (all origional)'!$AM$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'forecasts (all origional)'!$AM$2:$AM$13</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'forecasts (all origional)'!$AN$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'forecasts (all origional)'!$AN$2:$AN$13</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="515">
   <si>
     <t>LTD</t>
   </si>
@@ -1610,6 +1601,9 @@
   </si>
   <si>
     <t>rmse</t>
+  </si>
+  <si>
+    <t>mape</t>
   </si>
 </sst>
 </file>
@@ -18045,7 +18039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AN23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AM1" sqref="AM1:AN13"/>
     </sheetView>
   </sheetViews>
@@ -18159,55 +18153,55 @@
         <v>857523939.624156</v>
       </c>
       <c r="AB2">
-        <f>(P2-O2)^2</f>
-        <v>2.2094984444063264E+16</v>
+        <f>ABS((P2-O2)/O2*100)</f>
+        <v>14.773263836146164</v>
       </c>
       <c r="AC2">
-        <f>(Q3-O3)^2</f>
-        <v>4857837675498577</v>
+        <f>ABS((Q3-O3)/O3*100)</f>
+        <v>7.9406732047670845</v>
       </c>
       <c r="AD2">
-        <f>(R4-O4)^2</f>
-        <v>507385084354952.88</v>
+        <f>ABS((R4-O4)/O4*100)</f>
+        <v>2.7620092202142397</v>
       </c>
       <c r="AE2">
-        <f>(S5-O5)^2</f>
-        <v>4338780777233769.5</v>
+        <f>ABS((S5-O5)/O5*100)</f>
+        <v>8.1020452147375845</v>
       </c>
       <c r="AF2">
-        <f>(T6-O6)^2</f>
-        <v>1.0044110160799018E+16</v>
+        <f>ABS((T6-O6)/O6*100)</f>
+        <v>15.075254589001236</v>
       </c>
       <c r="AG2">
-        <f>(U7-O7)^2</f>
-        <v>8167889999025034</v>
+        <f>ABS((U7-O7)/O7*100)</f>
+        <v>12.319324351985554</v>
       </c>
       <c r="AH2">
-        <f>(V8-O8)^2</f>
-        <v>2.1334774790545308E+16</v>
+        <f>ABS((V8-O8)/O8*100)</f>
+        <v>19.038045950417558</v>
       </c>
       <c r="AI2">
-        <f>(W9-O9)^2</f>
-        <v>2101704920430720.5</v>
+        <f>ABS((W9-O9)/O9*100)</f>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AJ2">
-        <f>(X10-O10)^2</f>
-        <v>1.927056348505044E+16</v>
+        <f>ABS((X10-O10)/O10*100)</f>
+        <v>24.262793459745112</v>
       </c>
       <c r="AK2">
-        <f>(Y11-O11)^2</f>
-        <v>1.9289902569993624E+16</v>
+        <f>ABS((Y11-O11)/O11*100)</f>
+        <v>18.104720779747797</v>
       </c>
       <c r="AL2">
-        <f>(Z12-O12)^2</f>
-        <v>5.6452628655759416E+16</v>
+        <f>ABS((Z12-O12)/O12*100)</f>
+        <v>42.219829747279618</v>
       </c>
       <c r="AM2">
         <v>1</v>
       </c>
       <c r="AN2">
-        <f>SQRT(AVERAGE(AB2:AL2))</f>
-        <v>123752157.94730213</v>
+        <f>AVERAGE(AB2:AL2)</f>
+        <v>15.687694073111247</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
@@ -18261,55 +18255,55 @@
         <v>808038345.82883704</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB13" si="0">(P3-O3)^2</f>
-        <v>4857837675498577</v>
+        <f t="shared" ref="AB3:AB13" si="0">ABS((P3-O3)/O3*100)</f>
+        <v>7.9406732047670845</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC13" si="1">(Q4-O4)^2</f>
-        <v>507385084354952.88</v>
+        <f t="shared" ref="AC3:AC13" si="1">ABS((Q4-O4)/O4*100)</f>
+        <v>2.7620092202142397</v>
       </c>
       <c r="AD3">
-        <f t="shared" ref="AD3:AD13" si="2">(R5-O5)^2</f>
-        <v>4338780777233769.5</v>
+        <f t="shared" ref="AD3:AD13" si="2">ABS((R5-O5)/O5*100)</f>
+        <v>8.1020452147375845</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE13" si="3">(S6-O6)^2</f>
-        <v>1.0044110160799018E+16</v>
+        <f t="shared" ref="AE3:AE13" si="3">ABS((S6-O6)/O6*100)</f>
+        <v>15.075254589001236</v>
       </c>
       <c r="AF3">
-        <f t="shared" ref="AF3:AF13" si="4">(T7-O7)^2</f>
-        <v>8167889999025034</v>
+        <f t="shared" ref="AF3:AF13" si="4">ABS((T7-O7)/O7*100)</f>
+        <v>12.319324351985554</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG13" si="5">(U8-O8)^2</f>
-        <v>2.1334774790545308E+16</v>
+        <f t="shared" ref="AG3:AG13" si="5">ABS((U8-O8)/O8*100)</f>
+        <v>19.038045950417558</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH13" si="6">(V9-O9)^2</f>
-        <v>2101704920430720.5</v>
+        <f t="shared" ref="AH3:AH13" si="6">ABS((V9-O9)/O9*100)</f>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AI3">
-        <f t="shared" ref="AI3:AI13" si="7">(W10-O10)^2</f>
-        <v>1.927056348505044E+16</v>
+        <f t="shared" ref="AI3:AI13" si="7">ABS((W10-O10)/O10*100)</f>
+        <v>24.262793459745112</v>
       </c>
       <c r="AJ3">
-        <f t="shared" ref="AJ3:AJ13" si="8">(X11-O11)^2</f>
-        <v>1.9289902569993624E+16</v>
+        <f t="shared" ref="AJ3:AJ13" si="8">ABS((X11-O11)/O11*100)</f>
+        <v>18.104720779747797</v>
       </c>
       <c r="AK3">
-        <f t="shared" ref="AK3:AK13" si="9">(Y12-O12)^2</f>
-        <v>5.6452628655759416E+16</v>
+        <f t="shared" ref="AK3:AK13" si="9">ABS((Y12-O12)/O12*100)</f>
+        <v>42.219829747279618</v>
       </c>
       <c r="AL3">
-        <f t="shared" ref="AL3:AL13" si="10">(Z13-O13)^2</f>
-        <v>6279539135964748</v>
+        <f t="shared" ref="AL3:AL13" si="10">ABS((Z13-O13)/O13*100)</f>
+        <v>10.209810573486298</v>
       </c>
       <c r="AM3">
         <v>2</v>
       </c>
       <c r="AN3">
-        <f t="shared" ref="AN3:AN13" si="11">SQRT(AVERAGE(AB3:AL3))</f>
-        <v>117799952.63722447</v>
+        <f t="shared" ref="AN3:AN13" si="11">AVERAGE(AB3:AL3)</f>
+        <v>15.272834685596713</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
@@ -18367,54 +18361,54 @@
       </c>
       <c r="AB4">
         <f t="shared" si="0"/>
-        <v>507385084354952.88</v>
+        <v>2.7620092202142397</v>
       </c>
       <c r="AC4">
         <f t="shared" si="1"/>
-        <v>4338780777233769.5</v>
+        <v>8.1020452147375845</v>
       </c>
       <c r="AD4">
         <f t="shared" si="2"/>
-        <v>1.0044110160799018E+16</v>
+        <v>15.075254589001236</v>
       </c>
       <c r="AE4">
         <f t="shared" si="3"/>
-        <v>8167889999025034</v>
+        <v>12.319324351985554</v>
       </c>
       <c r="AF4">
         <f t="shared" si="4"/>
-        <v>2.1334774790545308E+16</v>
+        <v>19.038045950417558</v>
       </c>
       <c r="AG4">
         <f t="shared" si="5"/>
-        <v>2101704920430720.5</v>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AH4">
         <f t="shared" si="6"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AI4">
         <f t="shared" si="7"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AJ4">
         <f t="shared" si="8"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AK4">
         <f t="shared" si="9"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AL4">
         <f t="shared" si="10"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AM4">
         <v>3</v>
       </c>
       <c r="AN4">
         <f t="shared" si="11"/>
-        <v>128344829.80404003</v>
+        <v>16.596014992362893</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
@@ -18475,54 +18469,54 @@
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>4338780777233769.5</v>
+        <v>8.1020452147375845</v>
       </c>
       <c r="AC5">
         <f t="shared" si="1"/>
-        <v>1.0044110160799018E+16</v>
+        <v>15.075254589001236</v>
       </c>
       <c r="AD5">
         <f t="shared" si="2"/>
-        <v>8167889999025034</v>
+        <v>12.319324351985554</v>
       </c>
       <c r="AE5">
         <f t="shared" si="3"/>
-        <v>2.1334774790545308E+16</v>
+        <v>19.038045950417558</v>
       </c>
       <c r="AF5">
         <f t="shared" si="4"/>
-        <v>2101704920430720.5</v>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AG5">
         <f t="shared" si="5"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AH5">
         <f t="shared" si="6"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AI5">
         <f t="shared" si="7"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="8"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AK5">
         <f t="shared" si="9"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AL5">
         <f t="shared" si="10"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AM5">
         <v>4</v>
       </c>
       <c r="AN5">
-        <f>SQRT(AVERAGE(AB5:AL5))</f>
-        <v>128777577.43114123</v>
+        <f t="shared" si="11"/>
+        <v>16.931568829750393</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
@@ -18586,54 +18580,54 @@
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>1.0044110160799018E+16</v>
+        <v>15.075254589001236</v>
       </c>
       <c r="AC6">
         <f t="shared" si="1"/>
-        <v>8167889999025034</v>
+        <v>12.319324351985554</v>
       </c>
       <c r="AD6">
         <f t="shared" si="2"/>
-        <v>2.1334774790545308E+16</v>
+        <v>19.038045950417558</v>
       </c>
       <c r="AE6">
         <f t="shared" si="3"/>
-        <v>2101704920430720.5</v>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AF6">
         <f t="shared" si="4"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AG6">
         <f t="shared" si="5"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AH6">
         <f t="shared" si="6"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AI6">
         <f t="shared" si="7"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="8"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AK6">
         <f t="shared" si="9"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AL6">
         <f t="shared" si="10"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AM6">
         <v>5</v>
       </c>
       <c r="AN6">
         <f t="shared" si="11"/>
-        <v>127318202.79778697</v>
+        <v>16.392843379263564</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
@@ -18700,54 +18694,54 @@
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>8167889999025034</v>
+        <v>12.319324351985554</v>
       </c>
       <c r="AC7">
         <f t="shared" si="1"/>
-        <v>2.1334774790545308E+16</v>
+        <v>19.038045950417558</v>
       </c>
       <c r="AD7">
         <f t="shared" si="2"/>
-        <v>2101704920430720.5</v>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AE7">
         <f t="shared" si="3"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AF7">
         <f t="shared" si="4"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AG7">
         <f t="shared" si="5"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AH7">
         <f t="shared" si="6"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AI7">
         <f t="shared" si="7"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="8"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AK7">
         <f t="shared" si="9"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AL7">
         <f t="shared" si="10"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AM7">
         <v>6</v>
       </c>
       <c r="AN7">
         <f t="shared" si="11"/>
-        <v>124789295.81019823</v>
+        <v>15.778277933352797</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
@@ -18817,54 +18811,54 @@
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>2.1334774790545308E+16</v>
+        <v>19.038045950417558</v>
       </c>
       <c r="AC8">
         <f t="shared" si="1"/>
-        <v>2101704920430720.5</v>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AD8">
         <f t="shared" si="2"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AE8">
         <f t="shared" si="3"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AF8">
         <f t="shared" si="4"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AG8">
         <f t="shared" si="5"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AH8">
         <f t="shared" si="6"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AI8">
         <f t="shared" si="7"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="8"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AK8">
         <f t="shared" si="9"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AL8">
         <f t="shared" si="10"/>
-        <v>1.021225126129745E+16</v>
+        <v>15.898961907234419</v>
       </c>
       <c r="AM8">
         <v>7</v>
       </c>
       <c r="AN8">
         <f t="shared" si="11"/>
-        <v>125531746.47334474</v>
+        <v>16.103699529284512</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -18937,54 +18931,54 @@
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>2101704920430720.5</v>
+        <v>7.9666744501817686</v>
       </c>
       <c r="AC9">
         <f t="shared" si="1"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AD9">
         <f t="shared" si="2"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AE9">
         <f t="shared" si="3"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AF9">
         <f t="shared" si="4"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AG9">
         <f t="shared" si="5"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AH9">
         <f t="shared" si="6"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AI9">
         <f t="shared" si="7"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AJ9">
         <f t="shared" si="8"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AK9">
         <f t="shared" si="9"/>
-        <v>1.021225126129745E+16</v>
+        <v>15.898961907234419</v>
       </c>
       <c r="AL9">
         <f t="shared" si="10"/>
-        <v>3368952011169172.5</v>
+        <v>8.2043643885249296</v>
       </c>
       <c r="AM9">
         <v>8</v>
       </c>
       <c r="AN9">
         <f t="shared" si="11"/>
-        <v>118848486.55469359</v>
+        <v>15.118819387294273</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
@@ -19060,54 +19054,54 @@
       </c>
       <c r="AB10">
         <f t="shared" si="0"/>
-        <v>1.927056348505044E+16</v>
+        <v>24.262793459745112</v>
       </c>
       <c r="AC10">
         <f t="shared" si="1"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AE10">
         <f t="shared" si="3"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AF10">
         <f t="shared" si="4"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AG10">
         <f t="shared" si="5"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AH10">
         <f t="shared" si="6"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AI10">
         <f t="shared" si="7"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="8"/>
-        <v>1.021225126129745E+16</v>
+        <v>15.898961907234419</v>
       </c>
       <c r="AK10">
         <f t="shared" si="9"/>
-        <v>3368952011169172.5</v>
+        <v>8.2043643885249296</v>
       </c>
       <c r="AL10">
         <f t="shared" si="10"/>
-        <v>4.1120595282682072E+16</v>
+        <v>22.320940972070161</v>
       </c>
       <c r="AM10">
         <v>9</v>
       </c>
       <c r="AN10">
         <f t="shared" si="11"/>
-        <v>132936581.14851211</v>
+        <v>16.423752707465948</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
@@ -19186,54 +19180,54 @@
       </c>
       <c r="AB11">
         <f t="shared" si="0"/>
-        <v>1.9289902569993624E+16</v>
+        <v>18.104720779747797</v>
       </c>
       <c r="AC11">
         <f t="shared" si="1"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AD11">
         <f t="shared" si="2"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AE11">
         <f t="shared" si="3"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AF11">
         <f t="shared" si="4"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AG11">
         <f t="shared" si="5"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AH11">
         <f t="shared" si="6"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AI11">
         <f t="shared" si="7"/>
-        <v>1.021225126129745E+16</v>
+        <v>15.898961907234419</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="8"/>
-        <v>3368952011169172.5</v>
+        <v>8.2043643885249296</v>
       </c>
       <c r="AK11">
         <f t="shared" si="9"/>
-        <v>4.1120595282682072E+16</v>
+        <v>22.320940972070161</v>
       </c>
       <c r="AL11">
         <f t="shared" si="10"/>
-        <v>6662075026279952</v>
+        <v>12.564587918179825</v>
       </c>
       <c r="AM11">
         <v>10</v>
       </c>
       <c r="AN11">
         <f t="shared" si="11"/>
-        <v>128553134.47726722</v>
+        <v>15.360279476414554</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
@@ -19315,54 +19309,54 @@
       </c>
       <c r="AB12">
         <f t="shared" si="0"/>
-        <v>5.6452628655759416E+16</v>
+        <v>42.219829747279618</v>
       </c>
       <c r="AC12">
         <f t="shared" si="1"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AD12">
         <f t="shared" si="2"/>
-        <v>3.3409069132551012E+16</v>
+        <v>22.495656579195082</v>
       </c>
       <c r="AE12">
         <f t="shared" si="3"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AF12">
         <f t="shared" si="4"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AG12">
         <f t="shared" si="5"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AH12">
         <f t="shared" si="6"/>
-        <v>1.021225126129745E+16</v>
+        <v>15.898961907234419</v>
       </c>
       <c r="AI12">
         <f t="shared" si="7"/>
-        <v>3368952011169172.5</v>
+        <v>8.2043643885249296</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="8"/>
-        <v>4.1120595282682072E+16</v>
+        <v>22.320940972070161</v>
       </c>
       <c r="AK12">
         <f t="shared" si="9"/>
-        <v>6662075026279952</v>
+        <v>12.564587918179825</v>
       </c>
       <c r="AL12">
         <f t="shared" si="10"/>
-        <v>1803258943324530.8</v>
+        <v>6.3433472553091796</v>
       </c>
       <c r="AM12">
         <v>11</v>
       </c>
       <c r="AN12">
         <f t="shared" si="11"/>
-        <v>122213802.44791755</v>
+        <v>14.291063701465589</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">
@@ -19443,54 +19437,54 @@
       </c>
       <c r="AB13">
         <f t="shared" si="0"/>
-        <v>6279539135964748</v>
+        <v>10.209810573486298</v>
       </c>
       <c r="AC13">
-        <f>(Q14-O14)^2</f>
-        <v>3.3409069132551012E+16</v>
+        <f t="shared" si="1"/>
+        <v>22.495656579195082</v>
       </c>
       <c r="AD13">
         <f t="shared" si="2"/>
-        <v>1731345312016256.5</v>
+        <v>6.4531014314767372</v>
       </c>
       <c r="AE13">
         <f t="shared" si="3"/>
-        <v>227644238106914.72</v>
+        <v>2.1760652593824679</v>
       </c>
       <c r="AF13">
         <f t="shared" si="4"/>
-        <v>3030989597413261.5</v>
+        <v>8.3150346839827769</v>
       </c>
       <c r="AG13">
         <f t="shared" si="5"/>
-        <v>1.021225126129745E+16</v>
+        <v>15.898961907234419</v>
       </c>
       <c r="AH13">
         <f t="shared" si="6"/>
-        <v>3368952011169172.5</v>
+        <v>8.2043643885249296</v>
       </c>
       <c r="AI13">
         <f t="shared" si="7"/>
-        <v>4.1120595282682072E+16</v>
+        <v>22.320940972070161</v>
       </c>
       <c r="AJ13">
         <f t="shared" si="8"/>
-        <v>6662075026279952</v>
+        <v>12.564587918179825</v>
       </c>
       <c r="AK13">
         <f t="shared" si="9"/>
-        <v>1803258943324530.8</v>
+        <v>6.3433472553091796</v>
       </c>
       <c r="AL13">
         <f t="shared" si="10"/>
-        <v>1.0521472812917694E+16</v>
+        <v>17.039562362151919</v>
       </c>
       <c r="AM13">
         <v>12</v>
       </c>
       <c r="AN13">
         <f t="shared" si="11"/>
-        <v>103733571.64728349</v>
+        <v>12.0019484846358</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.2">
@@ -20223,4 +20217,123 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EA255F-5E7D-0648-93C9-A7F997C4D7C0}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>15.687694073111247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>15.272834685596713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>16.596014992362893</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>16.931568829750393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>16.392843379263564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>15.778277933352797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>16.103699529284512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>15.118819387294273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>16.423752707465948</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>15.360279476414554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>14.291063701465589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12.0019484846358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>